<commit_message>
Post likes and post comments functionality
</commit_message>
<xml_diff>
--- a/MessengerAPIsDoc.xlsx
+++ b/MessengerAPIsDoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14420" tabRatio="500" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14420" tabRatio="500" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -830,7 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -1664,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
User Profile | user following and unfollowing system
</commit_message>
<xml_diff>
--- a/MessengerAPIsDoc.xlsx
+++ b/MessengerAPIsDoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="14420" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Forgot password 2" sheetId="12" r:id="rId11"/>
     <sheet name="Change password" sheetId="11" r:id="rId12"/>
     <sheet name="Get post comment list" sheetId="13" r:id="rId13"/>
+    <sheet name="User profile" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="74">
   <si>
     <t>Registration</t>
   </si>
@@ -238,6 +239,21 @@
   </si>
   <si>
     <t>Get post comment list</t>
+  </si>
+  <si>
+    <t>follower</t>
+  </si>
+  <si>
+    <t>following</t>
+  </si>
+  <si>
+    <t>User profile</t>
+  </si>
+  <si>
+    <t>/user-profile/:user_id</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
@@ -325,8 +341,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -376,7 +394,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -398,6 +416,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -419,6 +438,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1226,12 +1246,97 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:XFD2"/>
+    <mergeCell ref="A6:XFD6"/>
+    <mergeCell ref="A10:XFD10"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="T2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1487,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A13"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1571,6 +1676,38 @@
       </c>
       <c r="D13" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8">
+      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8">
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8">
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8">
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1800,7 +1937,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Get single post data
</commit_message>
<xml_diff>
--- a/MessengerAPIsDoc.xlsx
+++ b/MessengerAPIsDoc.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Get user" sheetId="3" r:id="rId3"/>
     <sheet name="Update user" sheetId="4" r:id="rId4"/>
-    <sheet name="Get post" sheetId="5" r:id="rId5"/>
+    <sheet name="Get posts" sheetId="5" r:id="rId5"/>
     <sheet name="Create post" sheetId="6" r:id="rId6"/>
     <sheet name="Like post" sheetId="7" r:id="rId7"/>
     <sheet name="Comment on post" sheetId="8" r:id="rId8"/>
@@ -22,6 +22,7 @@
     <sheet name="Get post comment list" sheetId="13" r:id="rId13"/>
     <sheet name="User profile" sheetId="14" r:id="rId14"/>
     <sheet name="User follow or un follow" sheetId="15" r:id="rId15"/>
+    <sheet name="Get post" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="83">
   <si>
     <t>Registration</t>
   </si>
@@ -279,6 +280,9 @@
   </si>
   <si>
     <t>User follow or un follow</t>
+  </si>
+  <si>
+    <t>/post/:post_id</t>
   </si>
 </sst>
 </file>
@@ -366,8 +370,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -427,7 +433,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -451,6 +457,7 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -474,6 +481,7 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1370,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1452,6 +1460,100 @@
       </c>
       <c r="B12" t="s">
         <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:XFD2"/>
+    <mergeCell ref="A6:XFD6"/>
+    <mergeCell ref="A10:XFD10"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1732,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Like post issue fixed
</commit_message>
<xml_diff>
--- a/MessengerAPIsDoc.xlsx
+++ b/MessengerAPIsDoc.xlsx
@@ -4,25 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Get user" sheetId="3" r:id="rId3"/>
     <sheet name="Update user" sheetId="4" r:id="rId4"/>
-    <sheet name="Get posts" sheetId="5" r:id="rId5"/>
-    <sheet name="Create post" sheetId="6" r:id="rId6"/>
-    <sheet name="Like post" sheetId="7" r:id="rId7"/>
-    <sheet name="Comment on post" sheetId="8" r:id="rId8"/>
-    <sheet name="Update comment on post" sheetId="9" r:id="rId9"/>
-    <sheet name="Forgot password 1" sheetId="10" r:id="rId10"/>
-    <sheet name="Forgot password 2" sheetId="12" r:id="rId11"/>
-    <sheet name="Change password" sheetId="11" r:id="rId12"/>
-    <sheet name="Get post comment list" sheetId="13" r:id="rId13"/>
-    <sheet name="User profile" sheetId="14" r:id="rId14"/>
-    <sheet name="User follow or un follow" sheetId="15" r:id="rId15"/>
-    <sheet name="Get post" sheetId="16" r:id="rId16"/>
+    <sheet name="Get post" sheetId="16" r:id="rId5"/>
+    <sheet name="Get posts" sheetId="5" r:id="rId6"/>
+    <sheet name="Create post" sheetId="6" r:id="rId7"/>
+    <sheet name="Like post" sheetId="7" r:id="rId8"/>
+    <sheet name="Comment on post" sheetId="8" r:id="rId9"/>
+    <sheet name="Update comment on post" sheetId="9" r:id="rId10"/>
+    <sheet name="Forgot password 1" sheetId="10" r:id="rId11"/>
+    <sheet name="Forgot password 2" sheetId="12" r:id="rId12"/>
+    <sheet name="Change password" sheetId="11" r:id="rId13"/>
+    <sheet name="Get post comment list" sheetId="13" r:id="rId14"/>
+    <sheet name="User profile" sheetId="14" r:id="rId15"/>
+    <sheet name="User follow or un follow" sheetId="15" r:id="rId16"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -919,6 +919,102 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:XFD2"/>
+    <mergeCell ref="A6:XFD6"/>
+    <mergeCell ref="A10:XFD10"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -996,7 +1092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -1077,102 +1173,6 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:XFD2"/>
-    <mergeCell ref="A6:XFD6"/>
-    <mergeCell ref="A10:XFD10"/>
-  </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1195,6 +1195,102 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:XFD2"/>
+    <mergeCell ref="A6:XFD6"/>
+    <mergeCell ref="A10:XFD10"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -1289,7 +1385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -1374,7 +1470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -1460,100 +1556,6 @@
       </c>
       <c r="B12" t="s">
         <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:XFD2"/>
-    <mergeCell ref="A6:XFD6"/>
-    <mergeCell ref="A10:XFD10"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1832,6 +1834,100 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:XFD2"/>
+    <mergeCell ref="A6:XFD6"/>
+    <mergeCell ref="A10:XFD10"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1948,113 +2044,6 @@
       </c>
       <c r="H22">
         <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:XFD2"/>
-    <mergeCell ref="A6:XFD6"/>
-    <mergeCell ref="A10:XFD10"/>
-  </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="36.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2076,17 +2065,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD14"/>
+      <selection sqref="A1:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -2099,7 +2087,7 @@
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2107,7 +2095,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -2141,18 +2129,28 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2177,14 +2175,14 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection sqref="A1:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -2197,7 +2195,7 @@
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2205,7 +2203,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -2239,7 +2237,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2266,16 +2270,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD15"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -2288,7 +2293,7 @@
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2299,7 +2304,7 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1">
@@ -2336,11 +2341,6 @@
     <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User followers and user followings
</commit_message>
<xml_diff>
--- a/MessengerAPIsDoc.xlsx
+++ b/MessengerAPIsDoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500" firstSheet="14" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="Get post comment list" sheetId="13" r:id="rId14"/>
     <sheet name="User profile" sheetId="14" r:id="rId15"/>
     <sheet name="User follow or un follow" sheetId="15" r:id="rId16"/>
+    <sheet name="Get user followers" sheetId="17" r:id="rId17"/>
+    <sheet name="Get user followings" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="86">
   <si>
     <t>Registration</t>
   </si>
@@ -177,12 +179,6 @@
     <t>is_liked</t>
   </si>
   <si>
-    <t>[0,1,false,true]</t>
-  </si>
-  <si>
-    <t>tinyint (bool)</t>
-  </si>
-  <si>
     <t>post_id</t>
   </si>
   <si>
@@ -283,6 +279,21 @@
   </si>
   <si>
     <t>/post/:post_id</t>
+  </si>
+  <si>
+    <t>Get user followers</t>
+  </si>
+  <si>
+    <t>&gt;= 0</t>
+  </si>
+  <si>
+    <t>/user/followings/:user_id?page=1&amp;page_size=10</t>
+  </si>
+  <si>
+    <t>/user/followers/:user_id?page=1&amp;page_size=10</t>
+  </si>
+  <si>
+    <t>&gt; 0</t>
   </si>
 </sst>
 </file>
@@ -370,8 +381,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -424,16 +443,16 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -458,6 +477,10 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -482,6 +505,10 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -828,8 +855,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -844,8 +871,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -857,8 +884,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="3" customFormat="1">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" s="5" customFormat="1">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -921,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection sqref="A1:XFD15"/>
     </sheetView>
   </sheetViews>
@@ -939,9 +966,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>55</v>
+    <row r="2" spans="1:4" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -949,14 +976,14 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -976,24 +1003,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1036,9 +1063,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>63</v>
+    <row r="2" spans="1:4" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1046,14 +1073,14 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1065,8 +1092,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="3" customFormat="1">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:4" s="5" customFormat="1">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1114,9 +1141,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>64</v>
+    <row r="2" spans="1:4" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1124,14 +1151,14 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1151,8 +1178,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1163,17 +1190,17 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1215,9 +1242,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>60</v>
+    <row r="2" spans="1:4" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1225,14 +1252,14 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1252,24 +1279,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1294,7 +1321,7 @@
   <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1313,9 +1340,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1">
-      <c r="A3" s="2" t="s">
-        <v>68</v>
+    <row r="3" spans="1:4" s="4" customFormat="1">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1323,14 +1350,14 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:4" s="5" customFormat="1">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1350,14 +1377,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="3" customFormat="1">
-      <c r="A11" s="3" t="s">
-        <v>67</v>
+    <row r="11" spans="1:4" s="5" customFormat="1">
+      <c r="A11" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1390,7 +1417,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1408,9 +1435,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>71</v>
+    <row r="2" spans="1:4" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1418,14 +1445,14 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1445,14 +1472,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1462,6 +1489,7 @@
     <mergeCell ref="A10:XFD10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1483,7 +1511,7 @@
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="36.5" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="5" max="5" width="33.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
@@ -1493,13 +1521,13 @@
       <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>81</v>
+      <c r="E1" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
@@ -1507,17 +1535,17 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1536,26 +1564,26 @@
       <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+      <c r="E8" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="E11" s="5" t="s">
-        <v>80</v>
+      <c r="E11" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1565,6 +1593,208 @@
     <mergeCell ref="A10:XFD10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:XFD2"/>
+    <mergeCell ref="A6:XFD6"/>
+    <mergeCell ref="A10:XFD10"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:XFD2"/>
+    <mergeCell ref="A6:XFD6"/>
+    <mergeCell ref="A10:XFD10"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1592,8 +1822,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1608,8 +1838,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1621,8 +1851,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="3" customFormat="1">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" s="5" customFormat="1">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1672,8 +1902,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1688,8 +1918,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1709,8 +1939,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1750,8 +1980,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1766,8 +1996,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1787,8 +2017,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1836,7 +2066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1861,8 +2091,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1871,14 +2101,14 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:6" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1898,14 +2128,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:6" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1956,8 +2186,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1972,8 +2202,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:6" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1993,8 +2223,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:6" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2016,10 +2246,10 @@
     </row>
     <row r="19" spans="7:8">
       <c r="G19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="7:8">
@@ -2085,8 +2315,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2101,8 +2331,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2122,8 +2352,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2175,7 +2405,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2193,9 +2423,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>50</v>
+    <row r="2" spans="1:4" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2209,8 +2439,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2230,8 +2460,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2240,15 +2470,12 @@
         <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2291,9 +2518,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>52</v>
+    <row r="2" spans="1:4" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2301,14 +2528,14 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2328,19 +2555,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" s="5" customFormat="1">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>